<commit_message>
Them danh sach dat phong, sanh sach phong. Mai lam lot.
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -187,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -357,6 +363,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +669,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +763,10 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">

</xml_diff>

<commit_message>
Them sua xoa cac phong
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -354,6 +354,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,8 +365,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +669,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,23 +685,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="E1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="J1" s="23" t="s">
+      <c r="H1" s="24"/>
+      <c r="J1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="24"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -763,10 +763,10 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -863,10 +863,10 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="26"/>
       <c r="J8" s="7" t="s">
         <v>19</v>
       </c>
@@ -895,10 +895,10 @@
       <c r="E10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
@@ -969,22 +969,22 @@
       <c r="E16" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="D18" s="23" t="s">
+      <c r="B18" s="26"/>
+      <c r="D18" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="G18" s="23" t="s">
+      <c r="E18" s="26"/>
+      <c r="G18" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="J18" s="23" t="s">
+      <c r="H18" s="26"/>
+      <c r="J18" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="24"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">

</xml_diff>

<commit_message>
Update lại database cho Hợp với Nhất
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
   <si>
     <t>nvarchar(100)</t>
   </si>
@@ -178,6 +178,66 @@
   </si>
   <si>
     <t>bit</t>
+  </si>
+  <si>
+    <t>users (Khách hàng)</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>news_cat_id</t>
+  </si>
+  <si>
+    <t>news_cat_name</t>
+  </si>
+  <si>
+    <t>news (Tin tức)</t>
+  </si>
+  <si>
+    <t>news_id</t>
+  </si>
+  <si>
+    <t>news_title</t>
+  </si>
+  <si>
+    <t>news_description</t>
+  </si>
+  <si>
+    <t>news_avatar</t>
+  </si>
+  <si>
+    <t>news_cat_description</t>
+  </si>
+  <si>
+    <t>nvarchar(255)</t>
+  </si>
+  <si>
+    <t>news_content</t>
+  </si>
+  <si>
+    <t>news_status</t>
+  </si>
+  <si>
+    <t>bit (Ẩn hay hiện tin)</t>
+  </si>
+  <si>
+    <t>contacts (Liên hệ)</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>news_categories (Danh mục tin tức)</t>
+  </si>
+  <si>
+    <t>Ẩn tin</t>
+  </si>
+  <si>
+    <t>Hiện tin</t>
   </si>
 </sst>
 </file>
@@ -193,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +326,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -331,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -358,17 +424,19 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,30 +752,30 @@
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="J1" s="25" t="s">
+      <c r="H1" s="28"/>
+      <c r="J1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="26"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -769,10 +837,10 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -869,10 +937,10 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="26"/>
+      <c r="E8" s="27"/>
       <c r="J8" s="7" t="s">
         <v>19</v>
       </c>
@@ -901,16 +969,16 @@
       <c r="E10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="26"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <v>0</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="20">
+        <v>0</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -925,12 +993,16 @@
       <c r="H11" s="18" t="s">
         <v>2</v>
       </c>
+      <c r="J11" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>1</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -944,6 +1016,12 @@
       </c>
       <c r="H12" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -953,6 +1031,12 @@
       <c r="E13" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="13" t="s">
@@ -969,28 +1053,58 @@
       <c r="E15" s="13" t="s">
         <v>33</v>
       </c>
+      <c r="G15" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="G16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="25" t="s">
+      <c r="B18" s="27"/>
+      <c r="D18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="G18" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="26"/>
-      <c r="J18" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="G18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -1005,17 +1119,11 @@
       <c r="E19" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>2</v>
+      <c r="J19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1031,14 +1139,8 @@
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>0</v>
@@ -1057,6 +1159,16 @@
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G21" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="J21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1071,6 +1183,12 @@
       <c r="E22" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="G22" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1085,6 +1203,12 @@
       <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
@@ -1093,6 +1217,16 @@
       <c r="B24" s="17" t="s">
         <v>2</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -1101,27 +1235,121 @@
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D25" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="G25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
+      <c r="D27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="G28" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G30" s="20">
+        <v>0</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G31" s="20">
+        <v>1</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Merger code, fix conflict update last
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -87,9 +87,6 @@
     <t>float</t>
   </si>
   <si>
-    <t>categories (Dịch vụ)</t>
-  </si>
-  <si>
     <t>cat_id</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Hiện tin</t>
+  </si>
+  <si>
+    <t>categories (Danh mục dịch vụ)</t>
   </si>
 </sst>
 </file>
@@ -430,13 +430,13 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,23 +759,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="26"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="28"/>
-      <c r="G1" s="28" t="s">
+      <c r="D1" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="J1" s="26" t="s">
+      <c r="H1" s="26"/>
+      <c r="J1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -806,13 +806,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -864,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>1</v>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>2</v>
@@ -937,10 +937,10 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="27"/>
+      <c r="D8" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="28"/>
       <c r="J8" s="7" t="s">
         <v>19</v>
       </c>
@@ -950,13 +950,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="D9" s="17" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>2</v>
@@ -969,20 +969,20 @@
       <c r="E10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>0</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2</v>
@@ -993,32 +993,32 @@
       <c r="H11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="27"/>
+      <c r="J11" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>1</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>2</v>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>0</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>22</v>
@@ -1048,53 +1048,53 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" s="27"/>
+      <c r="J16" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="D18" s="26" t="s">
+      <c r="A18" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="D18" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="28"/>
       <c r="G18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>0</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
@@ -1159,10 +1159,10 @@
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="27"/>
+      <c r="G21" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="28"/>
       <c r="J21" s="6" t="s">
         <v>16</v>
       </c>
@@ -1172,19 +1172,19 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>2</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>2</v>
@@ -1192,19 +1192,19 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>0</v>
@@ -1212,41 +1212,41 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="27"/>
+      <c r="J24" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="27"/>
+      <c r="D25" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="28"/>
       <c r="G25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>2</v>
@@ -1256,19 +1256,19 @@
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>0</v>
@@ -1278,13 +1278,13 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" s="24" t="s">
         <v>2</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>1</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J29" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1331,11 +1331,18 @@
         <v>1</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="D1:E1"/>
@@ -1343,13 +1350,6 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>